<commit_message>
Radio buttons are transformed to icons. PremiumCalculator excel works fine. Age is show only if the birthdate is not empty.
</commit_message>
<xml_diff>
--- a/Gergo_Ferenczy/AfterTrainingExcercise/UI Fields list AfterTrainingExcerciseGergő.xlsx
+++ b/Gergo_Ferenczy/AfterTrainingExcercise/UI Fields list AfterTrainingExcerciseGergő.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gergo\Desktop\AfterTrainingExcercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gergo\Documents\Git repos\Training_sandbox\Gergo_Ferenczy\AfterTrainingExcercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C0C62E-6E37-43A3-8DAC-398294BDFB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C21A15-C66F-41B5-BE92-FF41C2C21385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI Field List Specification" sheetId="1" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t>new, used</t>
+  </si>
+  <si>
+    <t>regular expression lesz a megoldás</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +686,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,7 +777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -825,6 +834,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1160,7 +1170,7 @@
   <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L24" sqref="L24:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2031,7 +2041,7 @@
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="8"/>
-      <c r="L24" t="s">
+      <c r="L24" s="22" t="s">
         <v>73</v>
       </c>
       <c r="M24" s="4"/>
@@ -2068,10 +2078,12 @@
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="8"/>
-      <c r="L25" t="s">
+      <c r="L25" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="8"/>
@@ -3226,6 +3238,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010099CDED3ECB2B4843831D8747C02ED9CF" ma:contentTypeVersion="10" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="76a815337efc6a58b2e8bd6b7d520bd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad" xmlns:ns3="c1503785-5146-4d31-9a3a-ab405e6c3296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae8f8b2acb53c9f89b3f048a00ead611" ns2:_="" ns3:_="">
     <xsd:import namespace="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad"/>
@@ -3428,15 +3449,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3444,6 +3456,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DA6FAC-CD55-4FF4-A70B-E9594B162970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D11A46C-97B6-4A4C-A3AD-0D9A4FDB3E7A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3458,14 +3478,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DA6FAC-CD55-4FF4-A70B-E9594B162970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changes in date, search - table view, Next buttons now validate.UI Field excel updated.
</commit_message>
<xml_diff>
--- a/Gergo_Ferenczy/AfterTrainingExcercise/UI Fields list AfterTrainingExcerciseGergő.xlsx
+++ b/Gergo_Ferenczy/AfterTrainingExcercise/UI Fields list AfterTrainingExcerciseGergő.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gergo\Documents\Git repos\Training_sandbox\Gergo_Ferenczy\AfterTrainingExcercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C21A15-C66F-41B5-BE92-FF41C2C21385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B96BE5-7B86-4A14-96C1-9C52A17340FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -475,19 +475,7 @@
     <t>CompletionMessages.SuccessMessage</t>
   </si>
   <si>
-    <t>Driver1</t>
-  </si>
-  <si>
-    <t>Driver2</t>
-  </si>
-  <si>
     <t>Calculated from ID 2</t>
-  </si>
-  <si>
-    <t>NoStyleGroup1</t>
-  </si>
-  <si>
-    <t>NoStyleGroup2</t>
   </si>
   <si>
     <t>For the Pricing factor Y/N - we do not know the formula, so we cannot be sure which attributes are pricing factors.</t>
@@ -516,9 +504,6 @@
     <t>Driver.FirstName</t>
   </si>
   <si>
-    <t>Driver2 - Address fieldset</t>
-  </si>
-  <si>
     <t>Driver.LastName</t>
   </si>
   <si>
@@ -547,13 +532,6 @@
     <t>ez a 2 attri együtt tud majd keresni CSV-ben</t>
   </si>
   <si>
-    <t>Driver1 - Address fieldset</t>
-  </si>
-  <si>
-    <t>How can we display a table with 3 column?
-SelectionTable attribute</t>
-  </si>
-  <si>
     <t xml:space="preserve">Is it okay to use Currency format for the ZH? Is there any better option?
 Container attribute will contain ZH and plate number, so it needs only 1 </t>
   </si>
@@ -565,6 +543,34 @@
   </si>
   <si>
     <t>regular expression lesz a megoldás</t>
+  </si>
+  <si>
+    <t>How can we display a table with 3 column?
+SelectionTable input type</t>
+  </si>
+  <si>
+    <t>Product.EndDate</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>StartDate + 1 year -1 day</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>CarSearch</t>
+  </si>
+  <si>
+    <t>RestOfCarInfo</t>
+  </si>
+  <si>
+    <t>Drivers panel</t>
+  </si>
+  <si>
+    <t>Drivers panel - Address fieldset</t>
   </si>
 </sst>
 </file>
@@ -828,13 +834,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1169,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24:L25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,25 +1256,25 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
     </row>
     <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -1276,7 +1282,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>61</v>
@@ -1309,7 +1315,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="11"/>
     </row>
@@ -1319,7 +1325,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>62</v>
@@ -1353,11 +1359,9 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>38</v>
@@ -1376,7 +1380,7 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1390,9 +1394,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
         <v>67</v>
       </c>
@@ -1411,7 +1413,7 @@
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1430,7 +1432,7 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>68</v>
@@ -1451,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="15" t="s">
@@ -1463,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="Q7" s="11"/>
     </row>
@@ -1473,7 +1475,7 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>63</v>
@@ -1494,7 +1496,7 @@
         <v>24</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -1512,7 +1514,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>64</v>
@@ -1551,7 +1553,7 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>65</v>
@@ -1588,7 +1590,7 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>66</v>
@@ -1627,7 +1629,7 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>69</v>
@@ -1654,7 +1656,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Q12" s="12"/>
     </row>
@@ -1663,9 +1665,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
         <v>70</v>
       </c>
@@ -1689,20 +1689,36 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="12"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1732,25 +1748,25 @@
       <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="22"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
@@ -1758,10 +1774,10 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>49</v>
@@ -1795,10 +1811,10 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>50</v>
@@ -1832,10 +1848,10 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>51</v>
@@ -1869,10 +1885,10 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>52</v>
@@ -1908,10 +1924,10 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>53</v>
@@ -1939,16 +1955,16 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>19</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>105</v>
+      <c r="C22" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>54</v>
@@ -1981,11 +1997,11 @@
         <v>20</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
-        <v>105</v>
+      <c r="C23" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>55</v>
@@ -2009,7 +2025,7 @@
         <v>17</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q23" s="11"/>
     </row>
@@ -2019,10 +2035,10 @@
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>49</v>
@@ -2041,7 +2057,7 @@
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="8"/>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="20" t="s">
         <v>73</v>
       </c>
       <c r="M24" s="4"/>
@@ -2056,10 +2072,10 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>50</v>
@@ -2078,11 +2094,11 @@
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="22" t="s">
+      <c r="L25" s="20" t="s">
         <v>73</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -2095,10 +2111,10 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>51</v>
@@ -2132,10 +2148,10 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>52</v>
@@ -2171,10 +2187,10 @@
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>53</v>
@@ -2202,16 +2218,16 @@
       <c r="P28" s="8"/>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>26</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>54</v>
@@ -2238,11 +2254,11 @@
         <v>27</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>95</v>
+      <c r="C30" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>55</v>
@@ -2266,7 +2282,7 @@
         <v>17</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q30" s="11"/>
     </row>
@@ -2299,7 +2315,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q31" s="11"/>
     </row>
@@ -2346,25 +2362,25 @@
       <c r="Q33" s="11"/>
     </row>
     <row r="34" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="22"/>
     </row>
     <row r="35" spans="1:17" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -3107,21 +3123,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3238,15 +3254,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010099CDED3ECB2B4843831D8747C02ED9CF" ma:contentTypeVersion="10" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="76a815337efc6a58b2e8bd6b7d520bd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad" xmlns:ns3="c1503785-5146-4d31-9a3a-ab405e6c3296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae8f8b2acb53c9f89b3f048a00ead611" ns2:_="" ns3:_="">
     <xsd:import namespace="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad"/>
@@ -3449,21 +3456,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DA6FAC-CD55-4FF4-A70B-E9594B162970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D11A46C-97B6-4A4C-A3AD-0D9A4FDB3E7A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3482,7 +3490,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C2522A-973B-457D-9E35-D7F6FF2370A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3497,4 +3505,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DA6FAC-CD55-4FF4-A70B-E9594B162970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>